<commit_message>
- changed target from blank to E. coli (is target organism mandatory?)
</commit_message>
<xml_diff>
--- a/JUMP Collection/JUMP Collection.xlsx
+++ b/JUMP Collection/JUMP Collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/JUMP Collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4883C6E6-590B-3D43-B78F-FFA803743975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80FAAC8-292B-054F-AA46-FB1BBE32D681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40700" yWindow="1820" windowWidth="42720" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48160" yWindow="2720" windowWidth="42720" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7768" uniqueCount="7647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7808" uniqueCount="7647">
   <si>
     <t>Collection Name</t>
   </si>
@@ -23899,8 +23899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15:I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24244,7 +24244,9 @@
         <v>7572</v>
       </c>
       <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
+      <c r="I15" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J15" s="18" t="b">
         <v>1</v>
       </c>
@@ -24276,7 +24278,9 @@
         <v>7573</v>
       </c>
       <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
+      <c r="I16" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J16" s="18" t="b">
         <v>1</v>
       </c>
@@ -24308,7 +24312,9 @@
         <v>7574</v>
       </c>
       <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
+      <c r="I17" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J17" s="18" t="b">
         <v>1</v>
       </c>
@@ -24340,7 +24346,9 @@
         <v>7575</v>
       </c>
       <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
+      <c r="I18" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J18" s="18" t="b">
         <v>1</v>
       </c>
@@ -24372,7 +24380,9 @@
         <v>7576</v>
       </c>
       <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
+      <c r="I19" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J19" s="18" t="b">
         <v>1</v>
       </c>
@@ -24404,7 +24414,9 @@
         <v>7577</v>
       </c>
       <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
+      <c r="I20" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J20" s="18" t="b">
         <v>1</v>
       </c>
@@ -24436,7 +24448,9 @@
         <v>7578</v>
       </c>
       <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
+      <c r="I21" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J21" s="18" t="b">
         <v>1</v>
       </c>
@@ -24468,7 +24482,9 @@
         <v>7579</v>
       </c>
       <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
+      <c r="I22" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J22" s="18" t="b">
         <v>1</v>
       </c>
@@ -24500,7 +24516,9 @@
         <v>7580</v>
       </c>
       <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
+      <c r="I23" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J23" s="18" t="b">
         <v>1</v>
       </c>
@@ -24532,7 +24550,9 @@
         <v>7581</v>
       </c>
       <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
+      <c r="I24" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J24" s="18" t="b">
         <v>1</v>
       </c>
@@ -24564,7 +24584,9 @@
         <v>7582</v>
       </c>
       <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
+      <c r="I25" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J25" s="18" t="b">
         <v>1</v>
       </c>
@@ -24596,7 +24618,9 @@
         <v>7583</v>
       </c>
       <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
+      <c r="I26" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J26" s="18" t="b">
         <v>1</v>
       </c>
@@ -24628,7 +24652,9 @@
         <v>7584</v>
       </c>
       <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
+      <c r="I27" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J27" s="18" t="b">
         <v>1</v>
       </c>
@@ -24660,7 +24686,9 @@
         <v>7585</v>
       </c>
       <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
+      <c r="I28" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J28" s="18" t="b">
         <v>1</v>
       </c>
@@ -24692,7 +24720,9 @@
         <v>7586</v>
       </c>
       <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
+      <c r="I29" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J29" s="18" t="b">
         <v>1</v>
       </c>
@@ -24724,7 +24754,9 @@
         <v>7587</v>
       </c>
       <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="I30" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J30" s="18" t="b">
         <v>1</v>
       </c>
@@ -24756,7 +24788,9 @@
         <v>7588</v>
       </c>
       <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
+      <c r="I31" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J31" s="18" t="b">
         <v>1</v>
       </c>
@@ -24788,7 +24822,9 @@
         <v>7589</v>
       </c>
       <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
+      <c r="I32" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J32" s="18" t="b">
         <v>1</v>
       </c>
@@ -24820,7 +24856,9 @@
         <v>7590</v>
       </c>
       <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
+      <c r="I33" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J33" s="18" t="b">
         <v>1</v>
       </c>
@@ -24852,7 +24890,9 @@
         <v>7591</v>
       </c>
       <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
+      <c r="I34" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J34" s="18" t="b">
         <v>1</v>
       </c>
@@ -24884,7 +24924,9 @@
         <v>7592</v>
       </c>
       <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
+      <c r="I35" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J35" s="18" t="b">
         <v>1</v>
       </c>
@@ -24916,7 +24958,9 @@
         <v>7593</v>
       </c>
       <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
+      <c r="I36" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J36" s="18" t="b">
         <v>0</v>
       </c>
@@ -24948,7 +24992,9 @@
         <v>7594</v>
       </c>
       <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
+      <c r="I37" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J37" s="18" t="b">
         <v>1</v>
       </c>
@@ -24980,7 +25026,9 @@
         <v>7595</v>
       </c>
       <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
+      <c r="I38" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J38" s="18" t="b">
         <v>0</v>
       </c>
@@ -25012,7 +25060,9 @@
         <v>7596</v>
       </c>
       <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
+      <c r="I39" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J39" s="18" t="b">
         <v>0</v>
       </c>
@@ -25044,7 +25094,9 @@
         <v>7597</v>
       </c>
       <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
+      <c r="I40" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J40" s="18" t="b">
         <v>1</v>
       </c>
@@ -25076,7 +25128,9 @@
         <v>7598</v>
       </c>
       <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
+      <c r="I41" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J41" s="18" t="b">
         <v>1</v>
       </c>
@@ -25108,7 +25162,9 @@
         <v>7599</v>
       </c>
       <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
+      <c r="I42" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J42" s="18" t="b">
         <v>1</v>
       </c>
@@ -25140,7 +25196,9 @@
         <v>7600</v>
       </c>
       <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
+      <c r="I43" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J43" s="18" t="b">
         <v>1</v>
       </c>
@@ -25172,7 +25230,9 @@
         <v>7601</v>
       </c>
       <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
+      <c r="I44" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J44" s="18" t="b">
         <v>1</v>
       </c>
@@ -25204,7 +25264,9 @@
         <v>7602</v>
       </c>
       <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
+      <c r="I45" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J45" s="18" t="b">
         <v>1</v>
       </c>
@@ -25236,7 +25298,9 @@
         <v>7603</v>
       </c>
       <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
+      <c r="I46" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J46" s="18" t="b">
         <v>1</v>
       </c>
@@ -25268,7 +25332,9 @@
         <v>7604</v>
       </c>
       <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
+      <c r="I47" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J47" s="18" t="b">
         <v>1</v>
       </c>
@@ -25300,7 +25366,9 @@
         <v>7605</v>
       </c>
       <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
+      <c r="I48" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J48" s="18" t="b">
         <v>1</v>
       </c>
@@ -25332,7 +25400,9 @@
         <v>7606</v>
       </c>
       <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
+      <c r="I49" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J49" s="18" t="b">
         <v>1</v>
       </c>
@@ -25364,7 +25434,9 @@
         <v>7607</v>
       </c>
       <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
+      <c r="I50" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J50" s="18" t="b">
         <v>1</v>
       </c>
@@ -25396,7 +25468,9 @@
         <v>7608</v>
       </c>
       <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
+      <c r="I51" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J51" s="18" t="b">
         <v>1</v>
       </c>
@@ -25428,7 +25502,9 @@
         <v>7609</v>
       </c>
       <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
+      <c r="I52" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J52" s="18" t="b">
         <v>1</v>
       </c>
@@ -25460,7 +25536,9 @@
         <v>7610</v>
       </c>
       <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
+      <c r="I53" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J53" s="18" t="b">
         <v>1</v>
       </c>
@@ -25492,7 +25570,9 @@
         <v>7611</v>
       </c>
       <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
+      <c r="I54" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J54" s="18" t="b">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
troubleshooting again - changed names and filenames with ' to prime
</commit_message>
<xml_diff>
--- a/JUMP Collection/JUMP Collection.xlsx
+++ b/JUMP Collection/JUMP Collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/JUMP Collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80FAAC8-292B-054F-AA46-FB1BBE32D681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25FEC72-495B-4645-BD2C-F295C19C55FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48160" yWindow="2720" windowWidth="42720" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37280" yWindow="2720" windowWidth="42720" windowHeight="18560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7808" uniqueCount="7647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7864" uniqueCount="7639">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22765,21 +22765,9 @@
     <t>pJUMP28-1A(sfGFP)</t>
   </si>
   <si>
-    <t>pJUMP27ts-1A(lacZ)</t>
-  </si>
-  <si>
     <t>pJUMP29-1A(lacZ)</t>
   </si>
   <si>
-    <t>pJUMP29[dCas9]-1A(lacZ)</t>
-  </si>
-  <si>
-    <t>pJUMP27ts[mCherry]-1A(lacZ)</t>
-  </si>
-  <si>
-    <t>pJUMP29-1D'(sfGFP)</t>
-  </si>
-  <si>
     <t>pJUMP29-1E(sfGFP)</t>
   </si>
   <si>
@@ -22816,9 +22804,6 @@
     <t>pJUMP48-2A(sfGFP)</t>
   </si>
   <si>
-    <t>pJUMP49-2D'(sfGFP)</t>
-  </si>
-  <si>
     <t>pJUMP49-2E(sfGFP)</t>
   </si>
   <si>
@@ -22885,21 +22870,9 @@
     <t>pJUMP28-1A(sfGFP).gb</t>
   </si>
   <si>
-    <t>pJUMP27ts-1A(lacZ).gb</t>
-  </si>
-  <si>
     <t>pJUMP29-1A(lacZ).gb</t>
   </si>
   <si>
-    <t>pJUMP29[dCas9]-1A(lacZ).gb</t>
-  </si>
-  <si>
-    <t>pJUMP27ts[mCherry]-1A(lacZ).gb</t>
-  </si>
-  <si>
-    <t>pJUMP29-1D'(sfGFP).gb</t>
-  </si>
-  <si>
     <t>pJUMP29-1E(sfGFP).gb</t>
   </si>
   <si>
@@ -22936,9 +22909,6 @@
     <t>pJUMP48-2A(sfGFP).gb</t>
   </si>
   <si>
-    <t>pJUMP49-2D'(sfGFP).gb</t>
-  </si>
-  <si>
     <t>pJUMP49-2E(sfGFP).gb</t>
   </si>
   <si>
@@ -22987,18 +22957,9 @@
     <t>Level 1 vector. sfGFP reporter. Origin pUC (high copy number)</t>
   </si>
   <si>
-    <t>Level 1 vector. With lacZ as alternative cloning reporter. Thermosensitive origin pSC101 (low copy number)</t>
-  </si>
-  <si>
     <t>Level 1 vector. With lacZ as alternative cloning reporter. OriV 9 (pBBR322/ROP; medium copy number).</t>
   </si>
   <si>
-    <t>Level 1 vector. With lacZ as alternative cloning reporter.OriV 9 (pBBR322/ROP; medium copy number). Constitutive dCas9 in downstream secondary site.</t>
-  </si>
-  <si>
-    <t>Level 1 vector. With lacZ as alternative cloning reporter. Thermosensitive origin pSC101 (low copy number). Constitutive mCherry in downstream secondary site.</t>
-  </si>
-  <si>
     <t>Level 1 vector. OriV 9 (pBBR322/ROP; medium copy number); sfGFP cloning reporter.</t>
   </si>
   <si>
@@ -23045,13 +23006,28 @@
   </si>
   <si>
     <t>Joint Universal Modular Plasmids (JUMP) is a modular vector platform for Golden Gate (PhytoBrick) and Biobrick assembly based on Standard European Vector Architecture (SEVA). The collection includes plasmids with 10 different replication origins allowing for flexibility in both copy number and chassis. A selection of the JUMP collection has been made available to iGEM teams through the iGEM 2022 Distribution. This collection was kindly provided under the OpenMTA by Marcos Valenzuela-Ortega at the French Lab, University of Edinburgh. For more information please see: Marcos Valenzuela-Ortega, Christopher French, Joint universal modular plasmids (JUMP): a flexible vector platform for synthetic biology, Synthetic Biology, Volume 6, Issue 1, 2021, ysab003, https://doi.org/10.1093/synbio/ysab003</t>
+  </si>
+  <si>
+    <t>Taken from https://doi.org/10.1093/synbio/ysab003</t>
+  </si>
+  <si>
+    <t>pJUMP29-1Dprime(sfGFP)</t>
+  </si>
+  <si>
+    <t>pJUMP49-2Dprime(sfGFP)</t>
+  </si>
+  <si>
+    <t>pJUMP49-2Dprime(sfGFP).gb</t>
+  </si>
+  <si>
+    <t>pJUMP29-1Dprime(sfGFP).gb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -23235,6 +23211,10 @@
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -23899,8 +23879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15:I54"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23924,7 +23904,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7644</v>
+        <v>7631</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4" t="s">
@@ -23938,7 +23918,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7645</v>
+        <v>7632</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -23975,7 +23955,7 @@
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
       <c r="A5" s="49" t="s">
-        <v>7646</v>
+        <v>7633</v>
       </c>
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
@@ -24232,23 +24212,27 @@
       <c r="B15" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+      <c r="C15" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E15" s="18" t="s">
-        <v>7612</v>
+        <v>7602</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>7572</v>
+        <v>7567</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J15" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" s="18" t="b">
         <v>1</v>
@@ -24266,23 +24250,27 @@
       <c r="B16" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="18"/>
+      <c r="C16" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E16" s="18" t="s">
-        <v>7613</v>
+        <v>7603</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>7573</v>
+        <v>7568</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J16" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" s="18" t="b">
         <v>1</v>
@@ -24300,23 +24288,27 @@
       <c r="B17" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="C17" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E17" s="18" t="s">
-        <v>7614</v>
+        <v>7604</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>7574</v>
+        <v>7569</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J17" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" s="18" t="b">
         <v>1</v>
@@ -24334,23 +24326,27 @@
       <c r="B18" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E18" s="18" t="s">
-        <v>7615</v>
+        <v>7605</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>7575</v>
+        <v>7570</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J18" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" s="18" t="b">
         <v>1</v>
@@ -24368,23 +24364,27 @@
       <c r="B19" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="20"/>
+      <c r="C19" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E19" s="18" t="s">
-        <v>7616</v>
+        <v>7606</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>7576</v>
+        <v>7571</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J19" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" s="18" t="b">
         <v>1</v>
@@ -24402,23 +24402,27 @@
       <c r="B20" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="20"/>
+      <c r="C20" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E20" s="18" t="s">
-        <v>7616</v>
+        <v>7606</v>
       </c>
       <c r="F20" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>7577</v>
+        <v>7572</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J20" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" s="18" t="b">
         <v>1</v>
@@ -24436,23 +24440,27 @@
       <c r="B21" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="20"/>
+      <c r="C21" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E21" s="18" t="s">
-        <v>7616</v>
+        <v>7606</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>7578</v>
+        <v>7573</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J21" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" s="18" t="b">
         <v>1</v>
@@ -24470,23 +24478,27 @@
       <c r="B22" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="C22" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E22" s="18" t="s">
-        <v>7616</v>
+        <v>7606</v>
       </c>
       <c r="F22" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>7579</v>
+        <v>7574</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J22" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" s="18" t="b">
         <v>1</v>
@@ -24504,23 +24516,27 @@
       <c r="B23" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
+      <c r="C23" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E23" s="18" t="s">
-        <v>7617</v>
+        <v>7607</v>
       </c>
       <c r="F23" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>7580</v>
+        <v>7575</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J23" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" s="18" t="b">
         <v>1</v>
@@ -24538,23 +24554,27 @@
       <c r="B24" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="20"/>
+      <c r="C24" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E24" s="18" t="s">
-        <v>7617</v>
+        <v>7607</v>
       </c>
       <c r="F24" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>7581</v>
+        <v>7576</v>
       </c>
       <c r="H24" s="18"/>
       <c r="I24" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J24" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24" s="18" t="b">
         <v>1</v>
@@ -24572,23 +24592,27 @@
       <c r="B25" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="20"/>
+      <c r="C25" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E25" s="18" t="s">
-        <v>7617</v>
+        <v>7607</v>
       </c>
       <c r="F25" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>7582</v>
+        <v>7577</v>
       </c>
       <c r="H25" s="18"/>
       <c r="I25" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J25" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" s="18" t="b">
         <v>1</v>
@@ -24606,23 +24630,27 @@
       <c r="B26" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="C26" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E26" s="18" t="s">
-        <v>7617</v>
+        <v>7607</v>
       </c>
       <c r="F26" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>7583</v>
+        <v>7578</v>
       </c>
       <c r="H26" s="18"/>
       <c r="I26" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J26" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" s="18" t="b">
         <v>1</v>
@@ -24640,23 +24668,27 @@
       <c r="B27" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="20"/>
+      <c r="C27" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E27" s="18" t="s">
-        <v>7618</v>
+        <v>7608</v>
       </c>
       <c r="F27" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>7584</v>
+        <v>7579</v>
       </c>
       <c r="H27" s="18"/>
       <c r="I27" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J27" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27" s="18" t="b">
         <v>1</v>
@@ -24674,23 +24706,27 @@
       <c r="B28" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="20"/>
+      <c r="C28" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E28" s="18" t="s">
-        <v>7619</v>
+        <v>7609</v>
       </c>
       <c r="F28" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>7585</v>
+        <v>7580</v>
       </c>
       <c r="H28" s="18"/>
       <c r="I28" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J28" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" s="18" t="b">
         <v>1</v>
@@ -24708,23 +24744,27 @@
       <c r="B29" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="20"/>
+      <c r="C29" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E29" s="18" t="s">
-        <v>7620</v>
+        <v>7610</v>
       </c>
       <c r="F29" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>7586</v>
+        <v>7581</v>
       </c>
       <c r="H29" s="18"/>
       <c r="I29" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J29" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29" s="18" t="b">
         <v>1</v>
@@ -24742,23 +24782,27 @@
       <c r="B30" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="20"/>
+      <c r="C30" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E30" s="18" t="s">
-        <v>7621</v>
+        <v>7611</v>
       </c>
       <c r="F30" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>7587</v>
+        <v>7582</v>
       </c>
       <c r="H30" s="18"/>
       <c r="I30" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J30" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K30" s="18" t="b">
         <v>1</v>
@@ -24776,23 +24820,27 @@
       <c r="B31" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="20"/>
+      <c r="C31" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E31" s="18" t="s">
-        <v>7622</v>
+        <v>7612</v>
       </c>
       <c r="F31" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>7588</v>
+        <v>7583</v>
       </c>
       <c r="H31" s="18"/>
       <c r="I31" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J31" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K31" s="18" t="b">
         <v>1</v>
@@ -24810,23 +24858,27 @@
       <c r="B32" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="20"/>
+      <c r="C32" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E32" s="18" t="s">
-        <v>7623</v>
+        <v>7613</v>
       </c>
       <c r="F32" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>7589</v>
+        <v>7584</v>
       </c>
       <c r="H32" s="18"/>
       <c r="I32" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J32" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" s="18" t="b">
         <v>1</v>
@@ -24844,23 +24896,27 @@
       <c r="B33" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="20"/>
+      <c r="C33" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E33" s="18" t="s">
-        <v>7624</v>
+        <v>7614</v>
       </c>
       <c r="F33" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>7590</v>
+        <v>7585</v>
       </c>
       <c r="H33" s="18"/>
       <c r="I33" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J33" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" s="18" t="b">
         <v>1</v>
@@ -24878,23 +24934,27 @@
       <c r="B34" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="20"/>
+      <c r="C34" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E34" s="18" t="s">
-        <v>7625</v>
+        <v>7615</v>
       </c>
       <c r="F34" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>7591</v>
+        <v>7586</v>
       </c>
       <c r="H34" s="18"/>
       <c r="I34" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J34" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34" s="18" t="b">
         <v>1</v>
@@ -24912,23 +24972,27 @@
       <c r="B35" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="20"/>
+      <c r="C35" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E35" s="18" t="s">
-        <v>7626</v>
+        <v>7616</v>
       </c>
       <c r="F35" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>7592</v>
+        <v>7587</v>
       </c>
       <c r="H35" s="18"/>
       <c r="I35" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J35" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35" s="18" t="b">
         <v>1</v>
@@ -24940,33 +25004,17 @@
       <c r="M35" s="21"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A36" s="41" t="s">
-        <v>7553</v>
-      </c>
-      <c r="B36" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="18" t="s">
-        <v>7627</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>7521</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>7593</v>
-      </c>
+      <c r="A36" s="41"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="20"/>
       <c r="H36" s="18"/>
-      <c r="I36" s="18" t="s">
-        <v>7419</v>
-      </c>
-      <c r="J36" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K36" s="18" t="b">
-        <v>1</v>
-      </c>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
       <c r="L36" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -24975,28 +25023,32 @@
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1">
       <c r="A37" s="41" t="s">
-        <v>7554</v>
+        <v>7553</v>
       </c>
       <c r="B37" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="20"/>
+      <c r="C37" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E37" s="18" t="s">
-        <v>7628</v>
+        <v>7617</v>
       </c>
       <c r="F37" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>7594</v>
+        <v>7588</v>
       </c>
       <c r="H37" s="18"/>
       <c r="I37" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J37" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" s="18" t="b">
         <v>1</v>
@@ -25008,33 +25060,17 @@
       <c r="M37" s="21"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A38" s="41" t="s">
-        <v>7555</v>
-      </c>
-      <c r="B38" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="18" t="s">
-        <v>7629</v>
-      </c>
-      <c r="F38" s="18" t="s">
-        <v>7521</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>7595</v>
-      </c>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="20"/>
       <c r="H38" s="18"/>
-      <c r="I38" s="18" t="s">
-        <v>7419</v>
-      </c>
-      <c r="J38" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K38" s="18" t="b">
-        <v>1</v>
-      </c>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
       <c r="L38" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -25042,33 +25078,17 @@
       <c r="M38" s="21"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A39" s="41" t="s">
-        <v>7556</v>
-      </c>
-      <c r="B39" s="41" t="s">
-        <v>53</v>
-      </c>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="18"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="18" t="s">
-        <v>7630</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>7521</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>7596</v>
-      </c>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="20"/>
       <c r="H39" s="18"/>
-      <c r="I39" s="18" t="s">
-        <v>7419</v>
-      </c>
-      <c r="J39" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K39" s="18" t="b">
-        <v>1</v>
-      </c>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
       <c r="L39" s="15">
         <f t="shared" ref="L39:L80" si="1">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M39,CHAR(160)," ")," ",""))))</f>
         <v>0</v>
@@ -25077,28 +25097,32 @@
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1">
       <c r="A40" s="41" t="s">
-        <v>7557</v>
+        <v>7635</v>
       </c>
       <c r="B40" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="20"/>
+      <c r="C40" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E40" s="18" t="s">
-        <v>7631</v>
+        <v>7618</v>
       </c>
       <c r="F40" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>7597</v>
+        <v>7638</v>
       </c>
       <c r="H40" s="18"/>
       <c r="I40" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J40" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40" s="18" t="b">
         <v>1</v>
@@ -25111,28 +25135,32 @@
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1">
       <c r="A41" s="41" t="s">
-        <v>7558</v>
+        <v>7554</v>
       </c>
       <c r="B41" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="20"/>
+      <c r="C41" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E41" s="18" t="s">
-        <v>7631</v>
+        <v>7618</v>
       </c>
       <c r="F41" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>7598</v>
+        <v>7589</v>
       </c>
       <c r="H41" s="18"/>
       <c r="I41" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J41" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41" s="18" t="b">
         <v>1</v>
@@ -25145,28 +25173,32 @@
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1">
       <c r="A42" s="41" t="s">
-        <v>7559</v>
+        <v>7555</v>
       </c>
       <c r="B42" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="18"/>
-      <c r="D42" s="20"/>
+      <c r="C42" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E42" s="18" t="s">
-        <v>7632</v>
+        <v>7619</v>
       </c>
       <c r="F42" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>7599</v>
+        <v>7590</v>
       </c>
       <c r="H42" s="18"/>
       <c r="I42" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J42" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42" s="18" t="b">
         <v>1</v>
@@ -25179,28 +25211,32 @@
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1">
       <c r="A43" s="41" t="s">
-        <v>7560</v>
+        <v>7556</v>
       </c>
       <c r="B43" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="18"/>
-      <c r="D43" s="20"/>
+      <c r="C43" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E43" s="18" t="s">
-        <v>7633</v>
+        <v>7620</v>
       </c>
       <c r="F43" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>7600</v>
+        <v>7591</v>
       </c>
       <c r="H43" s="18"/>
       <c r="I43" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J43" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K43" s="18" t="b">
         <v>1</v>
@@ -25213,28 +25249,32 @@
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1">
       <c r="A44" s="41" t="s">
-        <v>7561</v>
+        <v>7557</v>
       </c>
       <c r="B44" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="20"/>
+      <c r="C44" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E44" s="18" t="s">
-        <v>7634</v>
+        <v>7621</v>
       </c>
       <c r="F44" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G44" s="20" t="s">
-        <v>7601</v>
+        <v>7592</v>
       </c>
       <c r="H44" s="18"/>
       <c r="I44" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J44" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K44" s="18" t="b">
         <v>1</v>
@@ -25247,28 +25287,32 @@
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1">
       <c r="A45" s="41" t="s">
-        <v>7562</v>
+        <v>7558</v>
       </c>
       <c r="B45" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="20"/>
+      <c r="C45" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E45" s="18" t="s">
-        <v>7635</v>
+        <v>7622</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G45" s="20" t="s">
-        <v>7602</v>
+        <v>7593</v>
       </c>
       <c r="H45" s="18"/>
       <c r="I45" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J45" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K45" s="18" t="b">
         <v>1</v>
@@ -25281,28 +25325,32 @@
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1">
       <c r="A46" s="41" t="s">
-        <v>7563</v>
+        <v>7559</v>
       </c>
       <c r="B46" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="20"/>
+      <c r="C46" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E46" s="18" t="s">
-        <v>7636</v>
+        <v>7623</v>
       </c>
       <c r="F46" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>7603</v>
+        <v>7594</v>
       </c>
       <c r="H46" s="18"/>
       <c r="I46" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J46" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K46" s="18" t="b">
         <v>1</v>
@@ -25315,28 +25363,32 @@
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1">
       <c r="A47" s="41" t="s">
-        <v>7564</v>
+        <v>7560</v>
       </c>
       <c r="B47" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="20"/>
+      <c r="C47" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E47" s="18" t="s">
-        <v>7637</v>
+        <v>7624</v>
       </c>
       <c r="F47" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G47" s="20" t="s">
-        <v>7604</v>
+        <v>7595</v>
       </c>
       <c r="H47" s="18"/>
       <c r="I47" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J47" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K47" s="18" t="b">
         <v>1</v>
@@ -25349,28 +25401,32 @@
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1">
       <c r="A48" s="41" t="s">
-        <v>7565</v>
+        <v>7561</v>
       </c>
       <c r="B48" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="20"/>
+      <c r="C48" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E48" s="18" t="s">
-        <v>7638</v>
+        <v>7625</v>
       </c>
       <c r="F48" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G48" s="20" t="s">
-        <v>7605</v>
+        <v>7596</v>
       </c>
       <c r="H48" s="18"/>
       <c r="I48" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J48" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K48" s="18" t="b">
         <v>1</v>
@@ -25383,28 +25439,32 @@
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1">
       <c r="A49" s="41" t="s">
-        <v>7566</v>
+        <v>7562</v>
       </c>
       <c r="B49" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C49" s="18"/>
-      <c r="D49" s="20"/>
+      <c r="C49" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E49" s="18" t="s">
-        <v>7639</v>
+        <v>7626</v>
       </c>
       <c r="F49" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G49" s="20" t="s">
-        <v>7606</v>
+        <v>7597</v>
       </c>
       <c r="H49" s="18"/>
       <c r="I49" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J49" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K49" s="18" t="b">
         <v>1</v>
@@ -25417,28 +25477,32 @@
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1">
       <c r="A50" s="41" t="s">
-        <v>7567</v>
+        <v>7563</v>
       </c>
       <c r="B50" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="20"/>
+      <c r="C50" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E50" s="18" t="s">
-        <v>7640</v>
+        <v>7627</v>
       </c>
       <c r="F50" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G50" s="20" t="s">
-        <v>7607</v>
+        <v>7598</v>
       </c>
       <c r="H50" s="18"/>
       <c r="I50" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J50" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K50" s="18" t="b">
         <v>1</v>
@@ -25451,28 +25515,32 @@
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1">
       <c r="A51" s="41" t="s">
-        <v>7568</v>
+        <v>7564</v>
       </c>
       <c r="B51" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="20"/>
+      <c r="C51" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E51" s="18" t="s">
-        <v>7641</v>
+        <v>7628</v>
       </c>
       <c r="F51" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G51" s="20" t="s">
-        <v>7608</v>
+        <v>7599</v>
       </c>
       <c r="H51" s="18"/>
       <c r="I51" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J51" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K51" s="18" t="b">
         <v>1</v>
@@ -25485,28 +25553,32 @@
     </row>
     <row r="52" spans="1:13" ht="15.75" customHeight="1">
       <c r="A52" s="41" t="s">
-        <v>7569</v>
+        <v>7565</v>
       </c>
       <c r="B52" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C52" s="18"/>
-      <c r="D52" s="20"/>
+      <c r="C52" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E52" s="18" t="s">
-        <v>7642</v>
+        <v>7629</v>
       </c>
       <c r="F52" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G52" s="20" t="s">
-        <v>7609</v>
+        <v>7600</v>
       </c>
       <c r="H52" s="18"/>
       <c r="I52" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J52" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K52" s="18" t="b">
         <v>1</v>
@@ -25519,28 +25591,32 @@
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1">
       <c r="A53" s="41" t="s">
-        <v>7570</v>
+        <v>7636</v>
       </c>
       <c r="B53" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="18"/>
-      <c r="D53" s="20"/>
+      <c r="C53" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E53" s="18" t="s">
-        <v>7643</v>
+        <v>7630</v>
       </c>
       <c r="F53" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G53" s="20" t="s">
-        <v>7610</v>
+        <v>7637</v>
       </c>
       <c r="H53" s="18"/>
       <c r="I53" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J53" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K53" s="18" t="b">
         <v>1</v>
@@ -25553,28 +25629,32 @@
     </row>
     <row r="54" spans="1:13" ht="15.75" customHeight="1">
       <c r="A54" s="41" t="s">
-        <v>7571</v>
+        <v>7566</v>
       </c>
       <c r="B54" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C54" s="18"/>
-      <c r="D54" s="20"/>
+      <c r="C54" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>7445</v>
+      </c>
       <c r="E54" s="18" t="s">
-        <v>7643</v>
+        <v>7630</v>
       </c>
       <c r="F54" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G54" s="20" t="s">
-        <v>7611</v>
+        <v>7601</v>
       </c>
       <c r="H54" s="18"/>
       <c r="I54" s="18" t="s">
         <v>7419</v>
       </c>
       <c r="J54" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K54" s="18" t="b">
         <v>1</v>
@@ -25595,12 +25675,8 @@
       <c r="G55" s="20"/>
       <c r="H55" s="18"/>
       <c r="I55" s="18"/>
-      <c r="J55" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K55" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
       <c r="L55" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25617,12 +25693,8 @@
       <c r="G56" s="20"/>
       <c r="H56" s="18"/>
       <c r="I56" s="18"/>
-      <c r="J56" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K56" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
       <c r="L56" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25639,12 +25711,8 @@
       <c r="G57" s="20"/>
       <c r="H57" s="18"/>
       <c r="I57" s="18"/>
-      <c r="J57" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K57" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
       <c r="L57" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25661,12 +25729,8 @@
       <c r="G58" s="20"/>
       <c r="H58" s="18"/>
       <c r="I58" s="18"/>
-      <c r="J58" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K58" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
       <c r="L58" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25683,12 +25747,8 @@
       <c r="G59" s="20"/>
       <c r="H59" s="18"/>
       <c r="I59" s="18"/>
-      <c r="J59" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K59" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J59" s="18"/>
+      <c r="K59" s="18"/>
       <c r="L59" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25705,12 +25765,8 @@
       <c r="G60" s="20"/>
       <c r="H60" s="18"/>
       <c r="I60" s="18"/>
-      <c r="J60" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K60" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
       <c r="L60" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25727,12 +25783,8 @@
       <c r="G61" s="20"/>
       <c r="H61" s="18"/>
       <c r="I61" s="18"/>
-      <c r="J61" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K61" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
       <c r="L61" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25749,12 +25801,8 @@
       <c r="G62" s="20"/>
       <c r="H62" s="18"/>
       <c r="I62" s="18"/>
-      <c r="J62" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K62" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J62" s="18"/>
+      <c r="K62" s="18"/>
       <c r="L62" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25771,12 +25819,8 @@
       <c r="G63" s="20"/>
       <c r="H63" s="18"/>
       <c r="I63" s="18"/>
-      <c r="J63" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K63" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J63" s="18"/>
+      <c r="K63" s="18"/>
       <c r="L63" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25793,12 +25837,8 @@
       <c r="G64" s="20"/>
       <c r="H64" s="18"/>
       <c r="I64" s="18"/>
-      <c r="J64" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K64" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J64" s="18"/>
+      <c r="K64" s="18"/>
       <c r="L64" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25815,12 +25855,8 @@
       <c r="G65" s="20"/>
       <c r="H65" s="18"/>
       <c r="I65" s="18"/>
-      <c r="J65" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K65" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
       <c r="L65" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25837,12 +25873,8 @@
       <c r="G66" s="20"/>
       <c r="H66" s="18"/>
       <c r="I66" s="18"/>
-      <c r="J66" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K66" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J66" s="18"/>
+      <c r="K66" s="18"/>
       <c r="L66" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25859,12 +25891,8 @@
       <c r="G67" s="20"/>
       <c r="H67" s="18"/>
       <c r="I67" s="18"/>
-      <c r="J67" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K67" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J67" s="18"/>
+      <c r="K67" s="18"/>
       <c r="L67" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25881,12 +25909,8 @@
       <c r="G68" s="20"/>
       <c r="H68" s="18"/>
       <c r="I68" s="18"/>
-      <c r="J68" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K68" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J68" s="18"/>
+      <c r="K68" s="18"/>
       <c r="L68" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25903,12 +25927,8 @@
       <c r="G69" s="20"/>
       <c r="H69" s="18"/>
       <c r="I69" s="18"/>
-      <c r="J69" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K69" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J69" s="18"/>
+      <c r="K69" s="18"/>
       <c r="L69" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25925,12 +25945,8 @@
       <c r="G70" s="20"/>
       <c r="H70" s="18"/>
       <c r="I70" s="18"/>
-      <c r="J70" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K70" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J70" s="18"/>
+      <c r="K70" s="18"/>
       <c r="L70" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25947,12 +25963,8 @@
       <c r="G71" s="20"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
-      <c r="J71" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K71" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J71" s="18"/>
+      <c r="K71" s="18"/>
       <c r="L71" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25969,12 +25981,8 @@
       <c r="G72" s="20"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
-      <c r="J72" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K72" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J72" s="18"/>
+      <c r="K72" s="18"/>
       <c r="L72" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25991,12 +25999,8 @@
       <c r="G73" s="20"/>
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
-      <c r="J73" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K73" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J73" s="18"/>
+      <c r="K73" s="18"/>
       <c r="L73" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -26013,12 +26017,8 @@
       <c r="G74" s="20"/>
       <c r="H74" s="18"/>
       <c r="I74" s="18"/>
-      <c r="J74" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K74" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J74" s="18"/>
+      <c r="K74" s="18"/>
       <c r="L74" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -26035,12 +26035,8 @@
       <c r="G75" s="20"/>
       <c r="H75" s="18"/>
       <c r="I75" s="18"/>
-      <c r="J75" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K75" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J75" s="18"/>
+      <c r="K75" s="18"/>
       <c r="L75" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -26057,12 +26053,8 @@
       <c r="G76" s="20"/>
       <c r="H76" s="18"/>
       <c r="I76" s="18"/>
-      <c r="J76" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K76" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J76" s="18"/>
+      <c r="K76" s="18"/>
       <c r="L76" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -26079,12 +26071,8 @@
       <c r="G77" s="20"/>
       <c r="H77" s="18"/>
       <c r="I77" s="18"/>
-      <c r="J77" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K77" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J77" s="18"/>
+      <c r="K77" s="18"/>
       <c r="L77" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -26101,12 +26089,8 @@
       <c r="G78" s="20"/>
       <c r="H78" s="18"/>
       <c r="I78" s="18"/>
-      <c r="J78" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K78" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J78" s="18"/>
+      <c r="K78" s="18"/>
       <c r="L78" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -26123,12 +26107,8 @@
       <c r="G79" s="20"/>
       <c r="H79" s="18"/>
       <c r="I79" s="18"/>
-      <c r="J79" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K79" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J79" s="18"/>
+      <c r="K79" s="18"/>
       <c r="L79" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -26145,12 +26125,8 @@
       <c r="G80" s="20"/>
       <c r="H80" s="18"/>
       <c r="I80" s="18"/>
-      <c r="J80" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K80" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="J80" s="18"/>
+      <c r="K80" s="18"/>
       <c r="L80" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -27064,6 +27040,7 @@
   <mergeCells count="1">
     <mergeCell ref="A5:F5"/>
   </mergeCells>
+  <phoneticPr fontId="28" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
troubleshooting - "Generate markdown for packages" issue with roles, changing plasmid -> plasmid_vector
</commit_message>
<xml_diff>
--- a/JUMP Collection/JUMP Collection.xlsx
+++ b/JUMP Collection/JUMP Collection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/JUMP Collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25FEC72-495B-4645-BD2C-F295C19C55FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4363A1DC-5369-A349-AED3-5A81EAC53E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37280" yWindow="2720" windowWidth="42720" windowHeight="18560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23879,8 +23879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24210,7 +24210,7 @@
         <v>7532</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>7634</v>
@@ -24248,7 +24248,7 @@
         <v>7533</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>7634</v>
@@ -24286,7 +24286,7 @@
         <v>7534</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>7634</v>
@@ -24324,7 +24324,7 @@
         <v>7535</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>7634</v>
@@ -24362,7 +24362,7 @@
         <v>7536</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>7634</v>
@@ -24400,7 +24400,7 @@
         <v>7537</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>7634</v>
@@ -24438,7 +24438,7 @@
         <v>7538</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>7634</v>
@@ -24476,7 +24476,7 @@
         <v>7539</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>7634</v>
@@ -24514,7 +24514,7 @@
         <v>7540</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>7634</v>
@@ -24552,7 +24552,7 @@
         <v>7541</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>7634</v>
@@ -24590,7 +24590,7 @@
         <v>7542</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>7634</v>
@@ -24628,7 +24628,7 @@
         <v>7543</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C26" s="21" t="s">
         <v>7634</v>
@@ -24666,7 +24666,7 @@
         <v>7544</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>7634</v>
@@ -24704,7 +24704,7 @@
         <v>7545</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>7634</v>
@@ -24742,7 +24742,7 @@
         <v>7546</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>7634</v>
@@ -24780,7 +24780,7 @@
         <v>7547</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C30" s="21" t="s">
         <v>7634</v>
@@ -24818,7 +24818,7 @@
         <v>7548</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>7634</v>
@@ -24856,7 +24856,7 @@
         <v>7549</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>7634</v>
@@ -24894,7 +24894,7 @@
         <v>7550</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>7634</v>
@@ -24932,7 +24932,7 @@
         <v>7551</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C34" s="21" t="s">
         <v>7634</v>
@@ -24970,7 +24970,7 @@
         <v>7552</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>7634</v>
@@ -25004,17 +25004,37 @@
       <c r="M35" s="21"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A36" s="41"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="20"/>
+      <c r="A36" s="41" t="s">
+        <v>7553</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>4473</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>7445</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>7617</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>7588</v>
+      </c>
       <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
+      <c r="I36" s="18" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J36" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" s="18" t="b">
+        <v>1</v>
+      </c>
       <c r="L36" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -25023,10 +25043,10 @@
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1">
       <c r="A37" s="41" t="s">
-        <v>7553</v>
+        <v>7635</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>7634</v>
@@ -25035,13 +25055,13 @@
         <v>7445</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>7617</v>
+        <v>7618</v>
       </c>
       <c r="F37" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>7588</v>
+        <v>7638</v>
       </c>
       <c r="H37" s="18"/>
       <c r="I37" s="18" t="s">
@@ -25060,17 +25080,37 @@
       <c r="M37" s="21"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="20"/>
+      <c r="A38" s="41" t="s">
+        <v>7554</v>
+      </c>
+      <c r="B38" s="41" t="s">
+        <v>4473</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>7445</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>7618</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>7589</v>
+      </c>
       <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
+      <c r="I38" s="18" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J38" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" s="18" t="b">
+        <v>1</v>
+      </c>
       <c r="L38" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -25078,17 +25118,37 @@
       <c r="M38" s="21"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="20"/>
+      <c r="A39" s="41" t="s">
+        <v>7555</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>4473</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>7634</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>7445</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>7619</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>7590</v>
+      </c>
       <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
+      <c r="I39" s="18" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J39" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K39" s="18" t="b">
+        <v>1</v>
+      </c>
       <c r="L39" s="15">
         <f t="shared" ref="L39:L80" si="1">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M39,CHAR(160)," ")," ",""))))</f>
         <v>0</v>
@@ -25097,10 +25157,10 @@
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1">
       <c r="A40" s="41" t="s">
-        <v>7635</v>
+        <v>7556</v>
       </c>
       <c r="B40" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>7634</v>
@@ -25109,13 +25169,13 @@
         <v>7445</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>7618</v>
+        <v>7620</v>
       </c>
       <c r="F40" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>7638</v>
+        <v>7591</v>
       </c>
       <c r="H40" s="18"/>
       <c r="I40" s="18" t="s">
@@ -25135,10 +25195,10 @@
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1">
       <c r="A41" s="41" t="s">
-        <v>7554</v>
+        <v>7557</v>
       </c>
       <c r="B41" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>7634</v>
@@ -25147,13 +25207,13 @@
         <v>7445</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>7618</v>
+        <v>7621</v>
       </c>
       <c r="F41" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>7589</v>
+        <v>7592</v>
       </c>
       <c r="H41" s="18"/>
       <c r="I41" s="18" t="s">
@@ -25173,10 +25233,10 @@
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1">
       <c r="A42" s="41" t="s">
-        <v>7555</v>
+        <v>7558</v>
       </c>
       <c r="B42" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>7634</v>
@@ -25185,13 +25245,13 @@
         <v>7445</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>7619</v>
+        <v>7622</v>
       </c>
       <c r="F42" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>7590</v>
+        <v>7593</v>
       </c>
       <c r="H42" s="18"/>
       <c r="I42" s="18" t="s">
@@ -25211,10 +25271,10 @@
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1">
       <c r="A43" s="41" t="s">
-        <v>7556</v>
+        <v>7559</v>
       </c>
       <c r="B43" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>7634</v>
@@ -25223,13 +25283,13 @@
         <v>7445</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>7620</v>
+        <v>7623</v>
       </c>
       <c r="F43" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>7591</v>
+        <v>7594</v>
       </c>
       <c r="H43" s="18"/>
       <c r="I43" s="18" t="s">
@@ -25249,10 +25309,10 @@
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1">
       <c r="A44" s="41" t="s">
-        <v>7557</v>
+        <v>7560</v>
       </c>
       <c r="B44" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C44" s="21" t="s">
         <v>7634</v>
@@ -25261,13 +25321,13 @@
         <v>7445</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>7621</v>
+        <v>7624</v>
       </c>
       <c r="F44" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G44" s="20" t="s">
-        <v>7592</v>
+        <v>7595</v>
       </c>
       <c r="H44" s="18"/>
       <c r="I44" s="18" t="s">
@@ -25287,10 +25347,10 @@
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1">
       <c r="A45" s="41" t="s">
-        <v>7558</v>
+        <v>7561</v>
       </c>
       <c r="B45" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>7634</v>
@@ -25299,13 +25359,13 @@
         <v>7445</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>7622</v>
+        <v>7625</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G45" s="20" t="s">
-        <v>7593</v>
+        <v>7596</v>
       </c>
       <c r="H45" s="18"/>
       <c r="I45" s="18" t="s">
@@ -25325,10 +25385,10 @@
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1">
       <c r="A46" s="41" t="s">
-        <v>7559</v>
+        <v>7562</v>
       </c>
       <c r="B46" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C46" s="21" t="s">
         <v>7634</v>
@@ -25337,13 +25397,13 @@
         <v>7445</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>7623</v>
+        <v>7626</v>
       </c>
       <c r="F46" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>7594</v>
+        <v>7597</v>
       </c>
       <c r="H46" s="18"/>
       <c r="I46" s="18" t="s">
@@ -25363,10 +25423,10 @@
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1">
       <c r="A47" s="41" t="s">
-        <v>7560</v>
+        <v>7563</v>
       </c>
       <c r="B47" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>7634</v>
@@ -25375,13 +25435,13 @@
         <v>7445</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>7624</v>
+        <v>7627</v>
       </c>
       <c r="F47" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G47" s="20" t="s">
-        <v>7595</v>
+        <v>7598</v>
       </c>
       <c r="H47" s="18"/>
       <c r="I47" s="18" t="s">
@@ -25401,10 +25461,10 @@
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1">
       <c r="A48" s="41" t="s">
-        <v>7561</v>
+        <v>7564</v>
       </c>
       <c r="B48" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C48" s="21" t="s">
         <v>7634</v>
@@ -25413,13 +25473,13 @@
         <v>7445</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>7625</v>
+        <v>7628</v>
       </c>
       <c r="F48" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G48" s="20" t="s">
-        <v>7596</v>
+        <v>7599</v>
       </c>
       <c r="H48" s="18"/>
       <c r="I48" s="18" t="s">
@@ -25439,10 +25499,10 @@
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1">
       <c r="A49" s="41" t="s">
-        <v>7562</v>
+        <v>7565</v>
       </c>
       <c r="B49" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>7634</v>
@@ -25451,13 +25511,13 @@
         <v>7445</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>7626</v>
+        <v>7629</v>
       </c>
       <c r="F49" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G49" s="20" t="s">
-        <v>7597</v>
+        <v>7600</v>
       </c>
       <c r="H49" s="18"/>
       <c r="I49" s="18" t="s">
@@ -25477,10 +25537,10 @@
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1">
       <c r="A50" s="41" t="s">
-        <v>7563</v>
+        <v>7636</v>
       </c>
       <c r="B50" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C50" s="21" t="s">
         <v>7634</v>
@@ -25489,13 +25549,13 @@
         <v>7445</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>7627</v>
+        <v>7630</v>
       </c>
       <c r="F50" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G50" s="20" t="s">
-        <v>7598</v>
+        <v>7637</v>
       </c>
       <c r="H50" s="18"/>
       <c r="I50" s="18" t="s">
@@ -25515,10 +25575,10 @@
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1">
       <c r="A51" s="41" t="s">
-        <v>7564</v>
+        <v>7566</v>
       </c>
       <c r="B51" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>7634</v>
@@ -25527,13 +25587,13 @@
         <v>7445</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>7628</v>
+        <v>7630</v>
       </c>
       <c r="F51" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G51" s="20" t="s">
-        <v>7599</v>
+        <v>7601</v>
       </c>
       <c r="H51" s="18"/>
       <c r="I51" s="18" t="s">
@@ -25552,37 +25612,17 @@
       <c r="M51" s="24"/>
     </row>
     <row r="52" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A52" s="41" t="s">
-        <v>7565</v>
-      </c>
-      <c r="B52" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>7634</v>
-      </c>
-      <c r="D52" s="18" t="s">
-        <v>7445</v>
-      </c>
-      <c r="E52" s="18" t="s">
-        <v>7629</v>
-      </c>
-      <c r="F52" s="18" t="s">
-        <v>7521</v>
-      </c>
-      <c r="G52" s="20" t="s">
-        <v>7600</v>
-      </c>
+      <c r="A52" s="41"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="20"/>
       <c r="H52" s="18"/>
-      <c r="I52" s="18" t="s">
-        <v>7419</v>
-      </c>
-      <c r="J52" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K52" s="18" t="b">
-        <v>1</v>
-      </c>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
       <c r="L52" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25590,37 +25630,17 @@
       <c r="M52" s="21"/>
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A53" s="41" t="s">
-        <v>7636</v>
-      </c>
-      <c r="B53" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>7634</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>7445</v>
-      </c>
-      <c r="E53" s="18" t="s">
-        <v>7630</v>
-      </c>
-      <c r="F53" s="18" t="s">
-        <v>7521</v>
-      </c>
-      <c r="G53" s="20" t="s">
-        <v>7637</v>
-      </c>
+      <c r="A53" s="41"/>
+      <c r="B53" s="41"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="20"/>
       <c r="H53" s="18"/>
-      <c r="I53" s="18" t="s">
-        <v>7419</v>
-      </c>
-      <c r="J53" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K53" s="18" t="b">
-        <v>1</v>
-      </c>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
       <c r="L53" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -25628,37 +25648,17 @@
       <c r="M53" s="21"/>
     </row>
     <row r="54" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A54" s="41" t="s">
-        <v>7566</v>
-      </c>
-      <c r="B54" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C54" s="21" t="s">
-        <v>7634</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>7445</v>
-      </c>
-      <c r="E54" s="18" t="s">
-        <v>7630</v>
-      </c>
-      <c r="F54" s="18" t="s">
-        <v>7521</v>
-      </c>
-      <c r="G54" s="20" t="s">
-        <v>7601</v>
-      </c>
+      <c r="A54" s="41"/>
+      <c r="B54" s="41"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="20"/>
       <c r="H54" s="18"/>
-      <c r="I54" s="18" t="s">
-        <v>7419</v>
-      </c>
-      <c r="J54" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K54" s="18" t="b">
-        <v>1</v>
-      </c>
+      <c r="I54" s="18"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
       <c r="L54" s="15">
         <f t="shared" si="1"/>
         <v>0</v>

</xml_diff>

<commit_message>
dealing with invalid characters - changed names in .xlsx to remove parenthesis - changed filenames in local folder to remove parenthesis - changed locus names in genbank files to remove parenthesis and apostrophe. did not change any other fields
</commit_message>
<xml_diff>
--- a/JUMP Collection/JUMP Collection.xlsx
+++ b/JUMP Collection/JUMP Collection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/JUMP Collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4363A1DC-5369-A349-AED3-5A81EAC53E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2E8A18-358F-BB44-9033-AB27F745FB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37280" yWindow="2720" windowWidth="42720" windowHeight="18560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22714,99 +22714,6 @@
     <t>pJUMP18-Uac</t>
   </si>
   <si>
-    <t>pJUMP29-1A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP29-1B(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP29-1C(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP29-1D(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP49-2A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP49-2B(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP49-2C(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP49-2D(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP21-1A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP22x-1A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP23-1A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP24-1A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP25-1A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP26-1A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP27-1A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP27ts-1A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP28-1A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP29-1A(lacZ)</t>
-  </si>
-  <si>
-    <t>pJUMP29-1E(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP39-1A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP38-1A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP41-2A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP42x-2A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP43-2A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP44-2A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP45-2A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP46-2A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP47-2A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP47ts-2A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP48-2A(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP49-2E(sfGFP)</t>
-  </si>
-  <si>
     <t>pJUMP19-min2.gb</t>
   </si>
   <si>
@@ -22819,99 +22726,6 @@
     <t>pJUMP18-Uac.gb</t>
   </si>
   <si>
-    <t>pJUMP29-1A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP29-1B(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP29-1C(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP29-1D(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP49-2A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP49-2B(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP49-2C(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP49-2D(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP21-1A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP22x-1A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP23-1A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP24-1A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP25-1A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP26-1A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP27-1A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP27ts-1A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP28-1A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP29-1A(lacZ).gb</t>
-  </si>
-  <si>
-    <t>pJUMP29-1E(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP39-1A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP38-1A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP41-2A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP42x-2A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP43-2A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP44-2A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP45-2A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP46-2A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP47-2A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP47ts-2A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP48-2A(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP49-2E(sfGFP).gb</t>
-  </si>
-  <si>
     <t>Minimal cargo vector. Allows introducing any part using BsmBI; but doesn't have cloning reporter. Can be used to generate new promoter/terminator acceptor vectors.</t>
   </si>
   <si>
@@ -23011,16 +22825,202 @@
     <t>Taken from https://doi.org/10.1093/synbio/ysab003</t>
   </si>
   <si>
-    <t>pJUMP29-1Dprime(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP49-2Dprime(sfGFP)</t>
-  </si>
-  <si>
-    <t>pJUMP49-2Dprime(sfGFP).gb</t>
-  </si>
-  <si>
-    <t>pJUMP29-1Dprime(sfGFP).gb</t>
+    <t>pJUMP29-1A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP29-1B-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP29-1C-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP29-1D-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP49-2A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP49-2B-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP49-2C-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP49-2D-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP21-1A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP22x-1A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP23-1A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP24-1A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP25-1A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP26-1A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP27-1A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP27ts-1A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP28-1A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP29-1Dprime-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP29-1E-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP39-1A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP38-1A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP41-2A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP42x-2A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP43-2A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP44-2A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP45-2A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP46-2A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP47-2A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP47ts-2A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP48-2A-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP49-2Dprime-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP49-2E-sfGFP</t>
+  </si>
+  <si>
+    <t>pJUMP29-1A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP29-1B-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP29-1C-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP29-1D-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP49-2A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP49-2B-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP49-2C-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP49-2D-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP21-1A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP22x-1A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP23-1A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP24-1A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP25-1A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP26-1A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP27-1A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP27ts-1A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP28-1A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP29-1Dprime-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP29-1E-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP39-1A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP38-1A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP41-2A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP42x-2A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP43-2A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP44-2A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP45-2A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP46-2A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP47-2A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP47ts-2A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP48-2A-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP49-2Dprime-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP49-2E-sfGFP.gb</t>
+  </si>
+  <si>
+    <t>pJUMP29-1A-lacZ</t>
+  </si>
+  <si>
+    <t>pJUMP29-1A-lacZ.gb</t>
   </si>
 </sst>
 </file>
@@ -23879,8 +23879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23904,7 +23904,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7631</v>
+        <v>7569</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4" t="s">
@@ -23918,7 +23918,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7632</v>
+        <v>7570</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -23955,7 +23955,7 @@
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
       <c r="A5" s="49" t="s">
-        <v>7633</v>
+        <v>7571</v>
       </c>
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
@@ -24213,19 +24213,19 @@
         <v>4473</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>7602</v>
+        <v>7540</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>7567</v>
+        <v>7536</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="18" t="s">
@@ -24251,19 +24251,19 @@
         <v>4473</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>7603</v>
+        <v>7541</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>7568</v>
+        <v>7537</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="18" t="s">
@@ -24289,19 +24289,19 @@
         <v>4473</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>7604</v>
+        <v>7542</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>7569</v>
+        <v>7538</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="18" t="s">
@@ -24327,19 +24327,19 @@
         <v>4473</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>7605</v>
+        <v>7543</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>7570</v>
+        <v>7539</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="18" t="s">
@@ -24359,25 +24359,25 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
       <c r="A19" s="18" t="s">
-        <v>7536</v>
+        <v>7573</v>
       </c>
       <c r="B19" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>7606</v>
+        <v>7544</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>7571</v>
+        <v>7605</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18" t="s">
@@ -24397,25 +24397,25 @@
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>7537</v>
+        <v>7574</v>
       </c>
       <c r="B20" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>7606</v>
+        <v>7544</v>
       </c>
       <c r="F20" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>7572</v>
+        <v>7606</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18" t="s">
@@ -24435,25 +24435,25 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" s="18" t="s">
-        <v>7538</v>
+        <v>7575</v>
       </c>
       <c r="B21" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>7606</v>
+        <v>7544</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>7573</v>
+        <v>7607</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18" t="s">
@@ -24473,25 +24473,25 @@
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>7539</v>
+        <v>7576</v>
       </c>
       <c r="B22" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>7606</v>
+        <v>7544</v>
       </c>
       <c r="F22" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>7574</v>
+        <v>7608</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18" t="s">
@@ -24511,25 +24511,25 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="A23" s="18" t="s">
-        <v>7540</v>
+        <v>7577</v>
       </c>
       <c r="B23" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>7607</v>
+        <v>7545</v>
       </c>
       <c r="F23" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>7575</v>
+        <v>7609</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18" t="s">
@@ -24549,25 +24549,25 @@
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>7541</v>
+        <v>7578</v>
       </c>
       <c r="B24" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>7607</v>
+        <v>7545</v>
       </c>
       <c r="F24" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>7576</v>
+        <v>7610</v>
       </c>
       <c r="H24" s="18"/>
       <c r="I24" s="18" t="s">
@@ -24587,25 +24587,25 @@
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>7542</v>
+        <v>7579</v>
       </c>
       <c r="B25" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>7607</v>
+        <v>7545</v>
       </c>
       <c r="F25" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>7577</v>
+        <v>7611</v>
       </c>
       <c r="H25" s="18"/>
       <c r="I25" s="18" t="s">
@@ -24625,25 +24625,25 @@
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
       <c r="A26" s="18" t="s">
-        <v>7543</v>
+        <v>7580</v>
       </c>
       <c r="B26" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>7607</v>
+        <v>7545</v>
       </c>
       <c r="F26" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>7578</v>
+        <v>7612</v>
       </c>
       <c r="H26" s="18"/>
       <c r="I26" s="18" t="s">
@@ -24663,25 +24663,25 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
       <c r="A27" s="18" t="s">
-        <v>7544</v>
+        <v>7581</v>
       </c>
       <c r="B27" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>7608</v>
+        <v>7546</v>
       </c>
       <c r="F27" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>7579</v>
+        <v>7613</v>
       </c>
       <c r="H27" s="18"/>
       <c r="I27" s="18" t="s">
@@ -24701,25 +24701,25 @@
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
       <c r="A28" s="41" t="s">
-        <v>7545</v>
+        <v>7582</v>
       </c>
       <c r="B28" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>7609</v>
+        <v>7547</v>
       </c>
       <c r="F28" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>7580</v>
+        <v>7614</v>
       </c>
       <c r="H28" s="18"/>
       <c r="I28" s="18" t="s">
@@ -24739,25 +24739,25 @@
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
       <c r="A29" s="41" t="s">
-        <v>7546</v>
+        <v>7583</v>
       </c>
       <c r="B29" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>7610</v>
+        <v>7548</v>
       </c>
       <c r="F29" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>7581</v>
+        <v>7615</v>
       </c>
       <c r="H29" s="18"/>
       <c r="I29" s="18" t="s">
@@ -24777,25 +24777,25 @@
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
       <c r="A30" s="41" t="s">
-        <v>7547</v>
+        <v>7584</v>
       </c>
       <c r="B30" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>7611</v>
+        <v>7549</v>
       </c>
       <c r="F30" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>7582</v>
+        <v>7616</v>
       </c>
       <c r="H30" s="18"/>
       <c r="I30" s="18" t="s">
@@ -24815,25 +24815,25 @@
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
       <c r="A31" s="41" t="s">
-        <v>7548</v>
+        <v>7585</v>
       </c>
       <c r="B31" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>7612</v>
+        <v>7550</v>
       </c>
       <c r="F31" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>7583</v>
+        <v>7617</v>
       </c>
       <c r="H31" s="18"/>
       <c r="I31" s="18" t="s">
@@ -24853,25 +24853,25 @@
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
       <c r="A32" s="41" t="s">
-        <v>7549</v>
+        <v>7586</v>
       </c>
       <c r="B32" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>7613</v>
+        <v>7551</v>
       </c>
       <c r="F32" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>7584</v>
+        <v>7618</v>
       </c>
       <c r="H32" s="18"/>
       <c r="I32" s="18" t="s">
@@ -24891,25 +24891,25 @@
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1">
       <c r="A33" s="41" t="s">
-        <v>7550</v>
+        <v>7587</v>
       </c>
       <c r="B33" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D33" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>7614</v>
+        <v>7552</v>
       </c>
       <c r="F33" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>7585</v>
+        <v>7619</v>
       </c>
       <c r="H33" s="18"/>
       <c r="I33" s="18" t="s">
@@ -24929,25 +24929,25 @@
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1">
       <c r="A34" s="41" t="s">
-        <v>7551</v>
+        <v>7588</v>
       </c>
       <c r="B34" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>7615</v>
+        <v>7553</v>
       </c>
       <c r="F34" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>7586</v>
+        <v>7620</v>
       </c>
       <c r="H34" s="18"/>
       <c r="I34" s="18" t="s">
@@ -24967,25 +24967,25 @@
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1">
       <c r="A35" s="41" t="s">
-        <v>7552</v>
+        <v>7589</v>
       </c>
       <c r="B35" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>7616</v>
+        <v>7554</v>
       </c>
       <c r="F35" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>7587</v>
+        <v>7621</v>
       </c>
       <c r="H35" s="18"/>
       <c r="I35" s="18" t="s">
@@ -25005,25 +25005,25 @@
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1">
       <c r="A36" s="41" t="s">
-        <v>7553</v>
+        <v>7637</v>
       </c>
       <c r="B36" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>7617</v>
+        <v>7555</v>
       </c>
       <c r="F36" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>7588</v>
+        <v>7638</v>
       </c>
       <c r="H36" s="18"/>
       <c r="I36" s="18" t="s">
@@ -25043,25 +25043,25 @@
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1">
       <c r="A37" s="41" t="s">
-        <v>7635</v>
+        <v>7590</v>
       </c>
       <c r="B37" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D37" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>7618</v>
+        <v>7556</v>
       </c>
       <c r="F37" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>7638</v>
+        <v>7622</v>
       </c>
       <c r="H37" s="18"/>
       <c r="I37" s="18" t="s">
@@ -25081,25 +25081,25 @@
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1">
       <c r="A38" s="41" t="s">
-        <v>7554</v>
+        <v>7591</v>
       </c>
       <c r="B38" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>7618</v>
+        <v>7556</v>
       </c>
       <c r="F38" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G38" s="20" t="s">
-        <v>7589</v>
+        <v>7623</v>
       </c>
       <c r="H38" s="18"/>
       <c r="I38" s="18" t="s">
@@ -25119,25 +25119,25 @@
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1">
       <c r="A39" s="41" t="s">
-        <v>7555</v>
+        <v>7592</v>
       </c>
       <c r="B39" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>7619</v>
+        <v>7557</v>
       </c>
       <c r="F39" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>7590</v>
+        <v>7624</v>
       </c>
       <c r="H39" s="18"/>
       <c r="I39" s="18" t="s">
@@ -25157,25 +25157,25 @@
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1">
       <c r="A40" s="41" t="s">
-        <v>7556</v>
+        <v>7593</v>
       </c>
       <c r="B40" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>7620</v>
+        <v>7558</v>
       </c>
       <c r="F40" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>7591</v>
+        <v>7625</v>
       </c>
       <c r="H40" s="18"/>
       <c r="I40" s="18" t="s">
@@ -25195,25 +25195,25 @@
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1">
       <c r="A41" s="41" t="s">
-        <v>7557</v>
+        <v>7594</v>
       </c>
       <c r="B41" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>7621</v>
+        <v>7559</v>
       </c>
       <c r="F41" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>7592</v>
+        <v>7626</v>
       </c>
       <c r="H41" s="18"/>
       <c r="I41" s="18" t="s">
@@ -25233,25 +25233,25 @@
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1">
       <c r="A42" s="41" t="s">
-        <v>7558</v>
+        <v>7595</v>
       </c>
       <c r="B42" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>7622</v>
+        <v>7560</v>
       </c>
       <c r="F42" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>7593</v>
+        <v>7627</v>
       </c>
       <c r="H42" s="18"/>
       <c r="I42" s="18" t="s">
@@ -25271,25 +25271,25 @@
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1">
       <c r="A43" s="41" t="s">
-        <v>7559</v>
+        <v>7596</v>
       </c>
       <c r="B43" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>7623</v>
+        <v>7561</v>
       </c>
       <c r="F43" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>7594</v>
+        <v>7628</v>
       </c>
       <c r="H43" s="18"/>
       <c r="I43" s="18" t="s">
@@ -25309,25 +25309,25 @@
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1">
       <c r="A44" s="41" t="s">
-        <v>7560</v>
+        <v>7597</v>
       </c>
       <c r="B44" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D44" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>7624</v>
+        <v>7562</v>
       </c>
       <c r="F44" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G44" s="20" t="s">
-        <v>7595</v>
+        <v>7629</v>
       </c>
       <c r="H44" s="18"/>
       <c r="I44" s="18" t="s">
@@ -25347,25 +25347,25 @@
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1">
       <c r="A45" s="41" t="s">
-        <v>7561</v>
+        <v>7598</v>
       </c>
       <c r="B45" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D45" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>7625</v>
+        <v>7563</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G45" s="20" t="s">
-        <v>7596</v>
+        <v>7630</v>
       </c>
       <c r="H45" s="18"/>
       <c r="I45" s="18" t="s">
@@ -25385,25 +25385,25 @@
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1">
       <c r="A46" s="41" t="s">
-        <v>7562</v>
+        <v>7599</v>
       </c>
       <c r="B46" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D46" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>7626</v>
+        <v>7564</v>
       </c>
       <c r="F46" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>7597</v>
+        <v>7631</v>
       </c>
       <c r="H46" s="18"/>
       <c r="I46" s="18" t="s">
@@ -25423,25 +25423,25 @@
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1">
       <c r="A47" s="41" t="s">
-        <v>7563</v>
+        <v>7600</v>
       </c>
       <c r="B47" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D47" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>7627</v>
+        <v>7565</v>
       </c>
       <c r="F47" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G47" s="20" t="s">
-        <v>7598</v>
+        <v>7632</v>
       </c>
       <c r="H47" s="18"/>
       <c r="I47" s="18" t="s">
@@ -25461,25 +25461,25 @@
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1">
       <c r="A48" s="41" t="s">
-        <v>7564</v>
+        <v>7601</v>
       </c>
       <c r="B48" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D48" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>7628</v>
+        <v>7566</v>
       </c>
       <c r="F48" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G48" s="20" t="s">
-        <v>7599</v>
+        <v>7633</v>
       </c>
       <c r="H48" s="18"/>
       <c r="I48" s="18" t="s">
@@ -25499,25 +25499,25 @@
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1">
       <c r="A49" s="41" t="s">
-        <v>7565</v>
+        <v>7602</v>
       </c>
       <c r="B49" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D49" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>7629</v>
+        <v>7567</v>
       </c>
       <c r="F49" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G49" s="20" t="s">
-        <v>7600</v>
+        <v>7634</v>
       </c>
       <c r="H49" s="18"/>
       <c r="I49" s="18" t="s">
@@ -25537,25 +25537,25 @@
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1">
       <c r="A50" s="41" t="s">
-        <v>7636</v>
+        <v>7603</v>
       </c>
       <c r="B50" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D50" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>7630</v>
+        <v>7568</v>
       </c>
       <c r="F50" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G50" s="20" t="s">
-        <v>7637</v>
+        <v>7635</v>
       </c>
       <c r="H50" s="18"/>
       <c r="I50" s="18" t="s">
@@ -25575,25 +25575,25 @@
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1">
       <c r="A51" s="41" t="s">
-        <v>7566</v>
+        <v>7604</v>
       </c>
       <c r="B51" s="41" t="s">
         <v>4473</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>7634</v>
+        <v>7572</v>
       </c>
       <c r="D51" s="18" t="s">
         <v>7445</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>7630</v>
+        <v>7568</v>
       </c>
       <c r="F51" s="18" t="s">
         <v>7521</v>
       </c>
       <c r="G51" s="20" t="s">
-        <v>7601</v>
+        <v>7636</v>
       </c>
       <c r="H51" s="18"/>
       <c r="I51" s="18" t="s">

</xml_diff>

<commit_message>
- changed back to final product -> true - changed back to role -> plasmid
</commit_message>
<xml_diff>
--- a/JUMP Collection/JUMP Collection.xlsx
+++ b/JUMP Collection/JUMP Collection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/JUMP Collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2E8A18-358F-BB44-9033-AB27F745FB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB949A4-1CC9-274E-8532-7947BA1794A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37280" yWindow="2720" windowWidth="42720" windowHeight="18560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23879,8 +23879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24210,7 +24210,7 @@
         <v>7532</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>7572</v>
@@ -24232,7 +24232,7 @@
         <v>7419</v>
       </c>
       <c r="J15" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="18" t="b">
         <v>1</v>
@@ -24248,7 +24248,7 @@
         <v>7533</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>7572</v>
@@ -24270,7 +24270,7 @@
         <v>7419</v>
       </c>
       <c r="J16" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="18" t="b">
         <v>1</v>
@@ -24286,7 +24286,7 @@
         <v>7534</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>7572</v>
@@ -24308,7 +24308,7 @@
         <v>7419</v>
       </c>
       <c r="J17" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="18" t="b">
         <v>1</v>
@@ -24324,7 +24324,7 @@
         <v>7535</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>7572</v>
@@ -24346,7 +24346,7 @@
         <v>7419</v>
       </c>
       <c r="J18" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="18" t="b">
         <v>1</v>
@@ -24362,7 +24362,7 @@
         <v>7573</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>7572</v>
@@ -24384,7 +24384,7 @@
         <v>7419</v>
       </c>
       <c r="J19" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="18" t="b">
         <v>1</v>
@@ -24400,7 +24400,7 @@
         <v>7574</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>7572</v>
@@ -24422,7 +24422,7 @@
         <v>7419</v>
       </c>
       <c r="J20" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="18" t="b">
         <v>1</v>
@@ -24438,7 +24438,7 @@
         <v>7575</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>7572</v>
@@ -24460,7 +24460,7 @@
         <v>7419</v>
       </c>
       <c r="J21" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="18" t="b">
         <v>1</v>
@@ -24476,7 +24476,7 @@
         <v>7576</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>7572</v>
@@ -24498,7 +24498,7 @@
         <v>7419</v>
       </c>
       <c r="J22" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="18" t="b">
         <v>1</v>
@@ -24514,7 +24514,7 @@
         <v>7577</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>7572</v>
@@ -24536,7 +24536,7 @@
         <v>7419</v>
       </c>
       <c r="J23" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="18" t="b">
         <v>1</v>
@@ -24552,7 +24552,7 @@
         <v>7578</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>7572</v>
@@ -24574,7 +24574,7 @@
         <v>7419</v>
       </c>
       <c r="J24" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="18" t="b">
         <v>1</v>
@@ -24590,7 +24590,7 @@
         <v>7579</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>7572</v>
@@ -24612,7 +24612,7 @@
         <v>7419</v>
       </c>
       <c r="J25" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="18" t="b">
         <v>1</v>
@@ -24628,7 +24628,7 @@
         <v>7580</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C26" s="21" t="s">
         <v>7572</v>
@@ -24650,7 +24650,7 @@
         <v>7419</v>
       </c>
       <c r="J26" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="18" t="b">
         <v>1</v>
@@ -24666,7 +24666,7 @@
         <v>7581</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>7572</v>
@@ -24688,7 +24688,7 @@
         <v>7419</v>
       </c>
       <c r="J27" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="18" t="b">
         <v>1</v>
@@ -24704,7 +24704,7 @@
         <v>7582</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>7572</v>
@@ -24726,7 +24726,7 @@
         <v>7419</v>
       </c>
       <c r="J28" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="18" t="b">
         <v>1</v>
@@ -24742,7 +24742,7 @@
         <v>7583</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>7572</v>
@@ -24764,7 +24764,7 @@
         <v>7419</v>
       </c>
       <c r="J29" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" s="18" t="b">
         <v>1</v>
@@ -24780,7 +24780,7 @@
         <v>7584</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C30" s="21" t="s">
         <v>7572</v>
@@ -24802,7 +24802,7 @@
         <v>7419</v>
       </c>
       <c r="J30" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="18" t="b">
         <v>1</v>
@@ -24818,7 +24818,7 @@
         <v>7585</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>7572</v>
@@ -24840,7 +24840,7 @@
         <v>7419</v>
       </c>
       <c r="J31" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" s="18" t="b">
         <v>1</v>
@@ -24856,7 +24856,7 @@
         <v>7586</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>7572</v>
@@ -24878,7 +24878,7 @@
         <v>7419</v>
       </c>
       <c r="J32" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32" s="18" t="b">
         <v>1</v>
@@ -24894,7 +24894,7 @@
         <v>7587</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>7572</v>
@@ -24916,7 +24916,7 @@
         <v>7419</v>
       </c>
       <c r="J33" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" s="18" t="b">
         <v>1</v>
@@ -24932,7 +24932,7 @@
         <v>7588</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C34" s="21" t="s">
         <v>7572</v>
@@ -24954,7 +24954,7 @@
         <v>7419</v>
       </c>
       <c r="J34" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" s="18" t="b">
         <v>1</v>
@@ -24970,7 +24970,7 @@
         <v>7589</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>7572</v>
@@ -24992,7 +24992,7 @@
         <v>7419</v>
       </c>
       <c r="J35" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="18" t="b">
         <v>1</v>
@@ -25008,7 +25008,7 @@
         <v>7637</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>7572</v>
@@ -25030,7 +25030,7 @@
         <v>7419</v>
       </c>
       <c r="J36" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="18" t="b">
         <v>1</v>
@@ -25046,7 +25046,7 @@
         <v>7590</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>7572</v>
@@ -25068,7 +25068,7 @@
         <v>7419</v>
       </c>
       <c r="J37" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" s="18" t="b">
         <v>1</v>
@@ -25084,7 +25084,7 @@
         <v>7591</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C38" s="21" t="s">
         <v>7572</v>
@@ -25106,7 +25106,7 @@
         <v>7419</v>
       </c>
       <c r="J38" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" s="18" t="b">
         <v>1</v>
@@ -25122,7 +25122,7 @@
         <v>7592</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>7572</v>
@@ -25144,7 +25144,7 @@
         <v>7419</v>
       </c>
       <c r="J39" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" s="18" t="b">
         <v>1</v>
@@ -25160,7 +25160,7 @@
         <v>7593</v>
       </c>
       <c r="B40" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>7572</v>
@@ -25182,7 +25182,7 @@
         <v>7419</v>
       </c>
       <c r="J40" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" s="18" t="b">
         <v>1</v>
@@ -25198,7 +25198,7 @@
         <v>7594</v>
       </c>
       <c r="B41" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>7572</v>
@@ -25220,7 +25220,7 @@
         <v>7419</v>
       </c>
       <c r="J41" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" s="18" t="b">
         <v>1</v>
@@ -25236,7 +25236,7 @@
         <v>7595</v>
       </c>
       <c r="B42" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>7572</v>
@@ -25258,7 +25258,7 @@
         <v>7419</v>
       </c>
       <c r="J42" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" s="18" t="b">
         <v>1</v>
@@ -25274,7 +25274,7 @@
         <v>7596</v>
       </c>
       <c r="B43" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>7572</v>
@@ -25296,7 +25296,7 @@
         <v>7419</v>
       </c>
       <c r="J43" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" s="18" t="b">
         <v>1</v>
@@ -25312,7 +25312,7 @@
         <v>7597</v>
       </c>
       <c r="B44" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C44" s="21" t="s">
         <v>7572</v>
@@ -25334,7 +25334,7 @@
         <v>7419</v>
       </c>
       <c r="J44" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" s="18" t="b">
         <v>1</v>
@@ -25350,7 +25350,7 @@
         <v>7598</v>
       </c>
       <c r="B45" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>7572</v>
@@ -25372,7 +25372,7 @@
         <v>7419</v>
       </c>
       <c r="J45" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45" s="18" t="b">
         <v>1</v>
@@ -25388,7 +25388,7 @@
         <v>7599</v>
       </c>
       <c r="B46" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C46" s="21" t="s">
         <v>7572</v>
@@ -25410,7 +25410,7 @@
         <v>7419</v>
       </c>
       <c r="J46" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K46" s="18" t="b">
         <v>1</v>
@@ -25426,7 +25426,7 @@
         <v>7600</v>
       </c>
       <c r="B47" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>7572</v>
@@ -25448,7 +25448,7 @@
         <v>7419</v>
       </c>
       <c r="J47" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47" s="18" t="b">
         <v>1</v>
@@ -25464,7 +25464,7 @@
         <v>7601</v>
       </c>
       <c r="B48" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C48" s="21" t="s">
         <v>7572</v>
@@ -25486,7 +25486,7 @@
         <v>7419</v>
       </c>
       <c r="J48" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K48" s="18" t="b">
         <v>1</v>
@@ -25502,7 +25502,7 @@
         <v>7602</v>
       </c>
       <c r="B49" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>7572</v>
@@ -25524,7 +25524,7 @@
         <v>7419</v>
       </c>
       <c r="J49" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K49" s="18" t="b">
         <v>1</v>
@@ -25540,7 +25540,7 @@
         <v>7603</v>
       </c>
       <c r="B50" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C50" s="21" t="s">
         <v>7572</v>
@@ -25562,7 +25562,7 @@
         <v>7419</v>
       </c>
       <c r="J50" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50" s="18" t="b">
         <v>1</v>
@@ -25578,7 +25578,7 @@
         <v>7604</v>
       </c>
       <c r="B51" s="41" t="s">
-        <v>4473</v>
+        <v>53</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>7572</v>
@@ -25600,7 +25600,7 @@
         <v>7419</v>
       </c>
       <c r="J51" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K51" s="18" t="b">
         <v>1</v>

</xml_diff>